<commit_message>
More detail added to example in score sheet
</commit_message>
<xml_diff>
--- a/Score Sheet.xlsx
+++ b/Score Sheet.xlsx
@@ -35,10 +35,10 @@
     <t>Score</t>
   </si>
   <si>
-    <t>Link without context</t>
+    <t>Home</t>
   </si>
   <si>
-    <t>Home</t>
+    <t>"Click Here" Link without context</t>
   </si>
 </sst>
 </file>
@@ -374,7 +374,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -397,10 +397,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>

</xml_diff>